<commit_message>
Update model for NMMPRC mtg Winnipeg
</commit_message>
<xml_diff>
--- a/data/Ages_sampled.xlsx
+++ b/data/Ages_sampled.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/26362cec7e0913ab/Documents/Nhydra/Projects/Harpseals/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/26362cec7e0913ab/Documents/Nhydra/Projects/Harpseals/HSmodel/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0F27ED7A-2D70-4AB2-828C-3BADD83120CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{0F27ED7A-2D70-4AB2-828C-3BADD83120CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9056567E-A93C-4BE5-BC45-8E3C7D383F7D}"/>
   <bookViews>
-    <workbookView xWindow="-24720" yWindow="1950" windowWidth="20640" windowHeight="12480" xr2:uid="{E3F39FE5-575D-42B4-891A-80E7B28E02A2}"/>
+    <workbookView xWindow="1785" yWindow="870" windowWidth="27015" windowHeight="15330" xr2:uid="{E3F39FE5-575D-42B4-891A-80E7B28E02A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -414,16 +414,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E5532A3-E30B-4F68-A6C3-0C38EC41E716}">
   <dimension ref="A1:AP37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="AQ1" sqref="AQ1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.64453125" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -551,7 +551,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -679,7 +679,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -807,7 +807,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -935,7 +935,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1063,7 +1063,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1191,7 +1191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1319,7 +1319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1447,7 +1447,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1575,7 +1575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1703,7 +1703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1831,7 +1831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1959,7 +1959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2087,7 +2087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2215,7 +2215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2343,7 +2343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2471,7 +2471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:42" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2599,7 +2599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:42" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2727,7 +2727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:42" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2855,7 +2855,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:42" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2983,7 +2983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:42" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3111,7 +3111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:42" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3239,7 +3239,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:42" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3367,7 +3367,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:42" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3495,7 +3495,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:42" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3623,7 +3623,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:42" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3751,7 +3751,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:42" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3879,7 +3879,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:42" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -4007,7 +4007,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:42" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -4135,7 +4135,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:42" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -4263,7 +4263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:42" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -4391,7 +4391,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:42" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -4519,7 +4519,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:42" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -4647,7 +4647,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:42" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -4775,7 +4775,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:42" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -4903,7 +4903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:42" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -5031,7 +5031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:42" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>

</xml_diff>